<commit_message>
tropopause detection from profile
</commit_message>
<xml_diff>
--- a/Tolten/Tolten_FlightTimes.xlsx
+++ b/Tolten/Tolten_FlightTimes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vandalsuidaho-my.sharepoint.com/personal/moon8435_vandals_uidaho_edu/Documents/%SummerInternship2020/hodographAnalysis/Tolten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{F29C345E-F78F-416E-89FB-72ADCFF6C2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBDBC87F-2B01-45BC-B602-1EF3DB40C6ED}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{F29C345E-F78F-416E-89FB-72ADCFF6C2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28C27883-C9A9-4CC1-B3A8-E8B6E61C1392}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{14FA5ADD-4B6E-4314-8BD2-80B808E68B12}"/>
   </bookViews>
@@ -66,7 +66,7 @@
     <t>[m]</t>
   </si>
   <si>
-    <t xml:space="preserve">Tropopause </t>
+    <t>Tropopause</t>
   </si>
 </sst>
 </file>
@@ -492,6 +492,9 @@
       <c r="D3" s="2">
         <v>0.66666666666666663</v>
       </c>
+      <c r="E3">
+        <v>12000</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -506,6 +509,9 @@
       <c r="D4" s="2">
         <v>0.70833333333333337</v>
       </c>
+      <c r="E4">
+        <v>12000</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -520,6 +526,9 @@
       <c r="D5" s="2">
         <v>0.75</v>
       </c>
+      <c r="E5">
+        <v>12000</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -534,6 +543,9 @@
       <c r="D6" s="2">
         <v>0.79166666666666696</v>
       </c>
+      <c r="E6">
+        <v>12000</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -548,6 +560,9 @@
       <c r="D7" s="2">
         <v>0.83333333333333304</v>
       </c>
+      <c r="E7">
+        <v>12000</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -562,6 +577,9 @@
       <c r="D8" s="2">
         <v>0.875</v>
       </c>
+      <c r="E8">
+        <v>12000</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -576,6 +594,9 @@
       <c r="D9" s="2">
         <v>0.91666666666666696</v>
       </c>
+      <c r="E9">
+        <v>12000</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -590,6 +611,9 @@
       <c r="D10" s="2">
         <v>0.95833333333333304</v>
       </c>
+      <c r="E10">
+        <v>12000</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -604,6 +628,9 @@
       <c r="D11" s="2">
         <v>0.999999999999998</v>
       </c>
+      <c r="E11">
+        <v>12000</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -618,6 +645,9 @@
       <c r="D12" s="2">
         <v>1.0416666666666601</v>
       </c>
+      <c r="E12">
+        <v>12000</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -632,6 +662,9 @@
       <c r="D13" s="2">
         <v>1.0833333333333299</v>
       </c>
+      <c r="E13">
+        <v>12000</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -646,6 +679,9 @@
       <c r="D14" s="2">
         <v>1.125</v>
       </c>
+      <c r="E14">
+        <v>12000</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -660,6 +696,9 @@
       <c r="D15" s="2">
         <v>1.1666666666666601</v>
       </c>
+      <c r="E15">
+        <v>12000</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -674,8 +713,11 @@
       <c r="D16" s="2">
         <v>1.2083333333333299</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -688,8 +730,11 @@
       <c r="D17" s="2">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -702,8 +747,11 @@
       <c r="D18" s="2">
         <v>1.2916666666666601</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -716,8 +764,11 @@
       <c r="D19" s="2">
         <v>1.3333333333333299</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -730,8 +781,11 @@
       <c r="D20" s="2">
         <v>1.375</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -744,8 +798,11 @@
       <c r="D21" s="2">
         <v>1.4166666666666601</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -758,8 +815,11 @@
       <c r="D22" s="2">
         <v>1.4583333333333299</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -772,8 +832,11 @@
       <c r="D23" s="2">
         <v>1.49999999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -786,8 +849,11 @@
       <c r="D24" s="2">
         <v>1.5416666666666601</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -800,8 +866,11 @@
       <c r="D25" s="2">
         <v>1.5833333333333299</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -814,8 +883,11 @@
       <c r="D26" s="2">
         <v>1.62499999999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -828,8 +900,11 @@
       <c r="D27" s="2">
         <v>0.64583333333333337</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -842,8 +917,11 @@
       <c r="D28" s="2">
         <v>0.6875</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -856,8 +934,11 @@
       <c r="D29" s="2">
         <v>0.72916666666666696</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -870,8 +951,11 @@
       <c r="D30" s="2">
         <v>0.77083333333333304</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -884,8 +968,11 @@
       <c r="D31" s="2">
         <v>0.8125</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -898,8 +985,11 @@
       <c r="D32" s="2">
         <v>0.85416666666666696</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -912,8 +1002,11 @@
       <c r="D33" s="2">
         <v>0.89583333333333304</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -926,8 +1019,11 @@
       <c r="D34" s="2">
         <v>0.9375</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -940,8 +1036,11 @@
       <c r="D35" s="2">
         <v>0.97916666666666596</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -954,8 +1053,11 @@
       <c r="D36" s="2">
         <v>1.0208333333333299</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -968,8 +1070,11 @@
       <c r="D37" s="2">
         <v>1.0625</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -982,8 +1087,11 @@
       <c r="D38" s="2">
         <v>1.1041666666666701</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -996,8 +1104,11 @@
       <c r="D39" s="2">
         <v>1.1458333333333299</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -1010,8 +1121,11 @@
       <c r="D40" s="2">
         <v>1.1875</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -1024,8 +1138,11 @@
       <c r="D41" s="2">
         <v>1.2291666666666701</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -1038,8 +1155,11 @@
       <c r="D42" s="2">
         <v>1.2708333333333299</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -1052,8 +1172,11 @@
       <c r="D43" s="2">
         <v>1.3125</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>8</v>
       </c>
@@ -1066,8 +1189,11 @@
       <c r="D44" s="2">
         <v>1.3541666666666701</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -1080,8 +1206,11 @@
       <c r="D45" s="2">
         <v>1.3958333333333299</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -1094,8 +1223,11 @@
       <c r="D46" s="2">
         <v>1.4375</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -1108,8 +1240,11 @@
       <c r="D47" s="2">
         <v>1.4791666666666701</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -1122,8 +1257,11 @@
       <c r="D48" s="2">
         <v>1.5208333333333299</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -1136,8 +1274,11 @@
       <c r="D49" s="2">
         <v>1.5625</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -1150,8 +1291,11 @@
       <c r="D50" s="2">
         <v>1.6041666666666701</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -1164,8 +1308,11 @@
       <c r="D51" s="2">
         <v>1.6458333333333299</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -1177,6 +1324,9 @@
       </c>
       <c r="D52" s="2">
         <v>1.6875</v>
+      </c>
+      <c r="E52">
+        <v>12000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>